<commit_message>
Hospitales nuevos and adjusted centroid
1- Fetch data for adjusted centroid municipios
2- Fetch data for hospitales nuevos
3- Bind adjusted centroid data with original
4- Adapt script to reproduce everything
</commit_message>
<xml_diff>
--- a/data/raw_data/hospitales.xlsx
+++ b/data/raw_data/hospitales.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/Desktop/r_projects/personal/transporte_hospitales/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Trabajo laptop\_personal\map_distance\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCD6E10-2D93-0A40-9CA4-FF48CF745C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE241962-61EF-48DE-9E6A-D90EE0449398}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24520" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="24525" windowHeight="16335" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="hospitales_existentes" sheetId="1" r:id="rId1"/>
+    <sheet name="hospitales_nuevos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -89,17 +90,45 @@
   </si>
   <si>
     <t>Hospital con área de shock</t>
+  </si>
+  <si>
+    <t>Hospital Traumatológico de San Cristobal</t>
+  </si>
+  <si>
+    <t>Hospital Municipal de Villa Altagracia</t>
+  </si>
+  <si>
+    <t>Hospital Provincial Leopoldo Martínez</t>
+  </si>
+  <si>
+    <t>Higuey</t>
+  </si>
+  <si>
+    <t>Hospital Regional Docente Taiwán 19 de Marzo</t>
+  </si>
+  <si>
+    <t>Hospital General Traumatológico en Sosúa</t>
+  </si>
+  <si>
+    <t>Hospital Municipal de Villa Vásquez</t>
+  </si>
+  <si>
+    <t>Hospital General Municipal de Miches</t>
+  </si>
+  <si>
+    <t>Hospital Regional Luis E. Bogaert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -113,6 +142,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0B57D0"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -136,9 +170,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -146,6 +180,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -446,21 +484,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.85546875" style="3"/>
+    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -480,7 +518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -500,7 +538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -520,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -540,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -560,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -580,7 +618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -600,7 +638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -620,7 +658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -640,7 +678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -660,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -680,7 +718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -700,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -720,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -740,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -760,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -784,4 +822,233 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CC07A7-7116-4E88-A47F-61DDEA1D2660}">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5">
+        <v>18.331544000000001</v>
+      </c>
+      <c r="D2" s="5">
+        <v>-70.156080000000003</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5">
+        <v>18.675174500000001</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-70.173255449999999</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5">
+        <v>18.761172395207101</v>
+      </c>
+      <c r="D4" s="5">
+        <v>-69.249964410000004</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5">
+        <v>18.616481</v>
+      </c>
+      <c r="D5" s="5">
+        <v>-68.711979999999997</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5">
+        <v>18.451111000000001</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-70.739016000000007</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5">
+        <v>19.750204530000001</v>
+      </c>
+      <c r="D7" s="5">
+        <v>-70.562043320000001</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="5">
+        <v>19.73692655</v>
+      </c>
+      <c r="D8" s="5">
+        <v>-71.443419109999994</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5">
+        <v>18.982164999999998</v>
+      </c>
+      <c r="D9" s="5">
+        <v>-69.044938999999999</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5">
+        <v>19.53915095</v>
+      </c>
+      <c r="D10" s="5">
+        <v>-71.081453589999995</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>